<commit_message>
Added Operating Systems Report. Just needs discussion on VMS and VMS excel tables.
</commit_message>
<xml_diff>
--- a/OpProject2.xlsx
+++ b/OpProject2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/779edd69e2276b4a/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayce\OneDrive\Desktop\os-proj2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{11CC4BFF-04CB-41BA-82C9-7325D3432BA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{E8D35D2C-07FD-45FB-9A86-FD11C2332819}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{11CC4BFF-04CB-41BA-82C9-7325D3432BA5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{9F98A6D9-202B-4A53-A1EB-C2A291097AE2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7D17D853-352F-4025-A4FC-7BF52474D8B6}"/>
   </bookViews>
@@ -147,7 +147,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>GCC.TACE</a:t>
+              <a:t>GCC.TRACE</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -517,7 +517,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$2</c15:sqref>
@@ -546,7 +546,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$3:$A$12</c15:sqref>
@@ -591,7 +591,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$3:$D$12</c15:sqref>
@@ -635,7 +635,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-FAA0-49FD-83D5-A955C6A055BC}"/>
                   </c:ext>
@@ -648,7 +648,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$2</c15:sqref>
@@ -677,7 +677,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$A$3:$A$12</c15:sqref>
@@ -722,7 +722,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$3:$E$12</c15:sqref>
@@ -766,7 +766,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-FAA0-49FD-83D5-A955C6A055BC}"/>
                   </c:ext>
@@ -5554,8 +5554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D948074-D844-4D0B-A1C3-E1C472539CEA}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>